<commit_message>
Update file format in Data folder
</commit_message>
<xml_diff>
--- a/Data/FileFormat.xlsx
+++ b/Data/FileFormat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zerox\Code\Visual Studio\source\repos\KTLT\LabProject\CSC10002-Course-Management\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zerox\Code\Visual Studio\source\repos\KTLT\LabProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA89AD6-D81A-43BA-943D-707F07E232B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B94BD7-6281-4520-A30E-A96BA11CE73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -53,9 +53,6 @@
     <t>2021_2022.txt; 2022_2023.txt</t>
   </si>
   <si>
-    <t>22CLC06.txt</t>
-  </si>
-  <si>
     <t>22CLC06_InputStud.csv</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>CSC10002_22CLC06_InputStud.csv</t>
   </si>
   <si>
-    <t>CSC10002_22CLC06_ImportScore.csv</t>
-  </si>
-  <si>
     <t>Import (Input) list of scoreboards to course(Course)</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>Input semester (Semester)</t>
   </si>
   <si>
-    <t>Input class (Class)</t>
-  </si>
-  <si>
     <t>InputSchoolYear (SchoolYear)</t>
   </si>
   <si>
@@ -98,9 +89,6 @@
     <t>start + "_" + (start + 1) + ".txt"</t>
   </si>
   <si>
-    <t>name + ".txt"</t>
-  </si>
-  <si>
     <t>name + "_InputStud.csv"</t>
   </si>
   <si>
@@ -113,9 +101,6 @@
     <t>ID + "_InputStud.csv"</t>
   </si>
   <si>
-    <t>ID + "_ImportScore.csv"</t>
-  </si>
-  <si>
     <t>Output list of students of course(Course)</t>
   </si>
   <si>
@@ -150,6 +135,207 @@
   </si>
   <si>
     <t>Input AcademicYear (AcademicYear)</t>
+  </si>
+  <si>
+    <t>File structure</t>
+  </si>
+  <si>
+    <t>List Of SchoolYear</t>
+  </si>
+  <si>
+    <t>ListSchoolYear.txt</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t>Number of classes</t>
+  </si>
+  <si>
+    <t>Number of schoolyears</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>name (Class)</t>
+  </si>
+  <si>
+    <t>"Class", name(Class)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Number of students", students.size() </t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>In4 of students</t>
+  </si>
+  <si>
+    <t>In4 of students (All in4 and score)</t>
+  </si>
+  <si>
+    <t>"ID", ID</t>
+  </si>
+  <si>
+    <t>"Name", name</t>
+  </si>
+  <si>
+    <t>"Gender", gender</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>"Dob", birth</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>"Social ID", socialID</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>Info of scoreboards</t>
+  </si>
+  <si>
+    <t>Output standard in4 of student(Student)</t>
+  </si>
+  <si>
+    <t>ID + "_OutputStdIn4.csv"</t>
+  </si>
+  <si>
+    <t>22127154_OutputStdIn4.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Class", name(Class) </t>
+  </si>
+  <si>
+    <t>*checkError*</t>
+  </si>
+  <si>
+    <t>start(SchoolYear)</t>
+  </si>
+  <si>
+    <t>List of AcademicYear</t>
+  </si>
+  <si>
+    <t>ListAcademicYear.txt</t>
+  </si>
+  <si>
+    <t>Number of AcademicYear</t>
+  </si>
+  <si>
+    <t>start(AcademicYear)</t>
+  </si>
+  <si>
+    <t>Number of semesters</t>
+  </si>
+  <si>
+    <t>semesterID</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>List of courseID</t>
+  </si>
+  <si>
+    <t>List of semesterID</t>
+  </si>
+  <si>
+    <t>courseID</t>
+  </si>
+  <si>
+    <t>classID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name  </t>
+  </si>
+  <si>
+    <t>teacher</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>L7</t>
+  </si>
+  <si>
+    <t>weekday</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>maxEnroll</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>ID + "_InputScore.csv"</t>
+  </si>
+  <si>
+    <t>CSC10002_22CLC06_InputScore.csv</t>
+  </si>
+  <si>
+    <t>L9</t>
+  </si>
+  <si>
+    <t>Number of students( number of scoreboards)</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>SchoolYear</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>AcademicYear</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Scoreboard</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Struct</t>
+  </si>
+  <si>
+    <t>For loop</t>
   </si>
 </sst>
 </file>
@@ -193,12 +379,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -481,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,154 +681,760 @@
     <col min="1" max="1" width="47.5546875" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="36.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" customWidth="1"/>
+    <col min="5" max="5" width="38.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" t="s">
+        <v>70</v>
+      </c>
+      <c r="G34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" t="s">
+        <v>70</v>
+      </c>
+      <c r="G38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" t="s">
+        <v>70</v>
+      </c>
+      <c r="G41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" t="s">
+        <v>70</v>
+      </c>
+      <c r="G42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" t="s">
+        <v>83</v>
+      </c>
+      <c r="F48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" t="s">
+        <v>81</v>
+      </c>
+      <c r="F49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>82</v>
+      </c>
+      <c r="E50" t="s">
+        <v>84</v>
+      </c>
+      <c r="F50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" t="s">
+        <v>57</v>
+      </c>
+      <c r="F52" t="s">
+        <v>89</v>
+      </c>
+      <c r="G52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B54" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C54" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
+      <c r="B55" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add number of course in Semester.txt
</commit_message>
<xml_diff>
--- a/Data/FileFormat.xlsx
+++ b/Data/FileFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zerox\Code\Visual Studio\source\repos\KTLT\LabProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B94BD7-6281-4520-A30E-A96BA11CE73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622F1FE1-D549-4696-86A4-57859F3D1FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>For loop</t>
+  </si>
+  <si>
+    <t>Number of courses</t>
   </si>
 </sst>
 </file>
@@ -379,15 +382,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -670,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,10 +701,10 @@
         <v>33</v>
       </c>
       <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1146,58 +1146,55 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
         <v>40</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>73</v>
       </c>
-      <c r="F34" t="s">
-        <v>70</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G35" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>12</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>19</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>8</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>39</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>75</v>
       </c>
-      <c r="F35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D36" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" t="s">
-        <v>76</v>
-      </c>
       <c r="F36" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F37" t="s">
         <v>70</v>
@@ -1208,10 +1205,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F38" t="s">
         <v>70</v>
@@ -1222,10 +1219,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F39" t="s">
         <v>70</v>
@@ -1236,10 +1233,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F40" t="s">
         <v>70</v>
@@ -1250,10 +1247,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E41" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F41" t="s">
         <v>70</v>
@@ -1264,10 +1261,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E42" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F42" t="s">
         <v>70</v>
@@ -1277,31 +1274,34 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="D43" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" t="s">
+        <v>84</v>
+      </c>
+      <c r="F43" t="s">
+        <v>70</v>
+      </c>
+      <c r="G43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>24</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>25</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>26</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>39</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>75</v>
-      </c>
-      <c r="F43" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D44" t="s">
-        <v>41</v>
-      </c>
-      <c r="E44" t="s">
-        <v>76</v>
       </c>
       <c r="F44" t="s">
         <v>62</v>
@@ -1309,10 +1309,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F45" t="s">
         <v>62</v>
@@ -1320,10 +1320,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F46" t="s">
         <v>62</v>
@@ -1331,10 +1331,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F47" t="s">
         <v>62</v>
@@ -1342,10 +1342,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E48" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F48" t="s">
         <v>62</v>
@@ -1353,10 +1353,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E49" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F49" t="s">
         <v>62</v>
@@ -1364,10 +1364,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E50" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F50" t="s">
         <v>62</v>
@@ -1375,59 +1375,70 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E51" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F51" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" t="s">
+        <v>88</v>
+      </c>
+      <c r="F52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
         <v>40</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>57</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F53" t="s">
         <v>89</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G53" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>11</v>
-      </c>
-      <c r="B53" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>10</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>85</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change format data, add new file Output list of students
</commit_message>
<xml_diff>
--- a/Data/FileFormat.xlsx
+++ b/Data/FileFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zerox\Code\Visual Studio\source\repos\KTLT\LabProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622F1FE1-D549-4696-86A4-57859F3D1FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CB0107-B6BD-477F-9A0D-EA858E594FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>Number of courses</t>
+  </si>
+  <si>
+    <t>"First name", first name</t>
+  </si>
+  <si>
+    <t>"Last name", last name</t>
   </si>
 </sst>
 </file>
@@ -670,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,7 +967,7 @@
         <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="F21" t="s">
         <v>70</v>
@@ -975,7 +981,7 @@
         <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="F22" t="s">
         <v>70</v>
@@ -989,7 +995,7 @@
         <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F23" t="s">
         <v>70</v>
@@ -1003,7 +1009,7 @@
         <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
         <v>70</v>
@@ -1017,128 +1023,131 @@
         <v>56</v>
       </c>
       <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" t="s">
         <v>61</v>
       </c>
-      <c r="F25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="F26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>64</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>65</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>36</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>39</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>66</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D27" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
         <v>40</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>67</v>
       </c>
-      <c r="F27" t="s">
-        <v>70</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>16</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>4</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>39</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>42</v>
       </c>
-      <c r="F28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D29" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" t="s">
-        <v>68</v>
-      </c>
       <c r="F29" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
         <v>40</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>74</v>
       </c>
-      <c r="F30" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>18</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>7</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>39</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>69</v>
       </c>
-      <c r="F31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D32" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" t="s">
-        <v>71</v>
-      </c>
       <c r="F32" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F33" t="s">
         <v>70</v>
@@ -1146,69 +1155,66 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E34" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="F34" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
         <v>40</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>73</v>
       </c>
-      <c r="F35" t="s">
-        <v>70</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="F36" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>12</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>19</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>8</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>39</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>75</v>
       </c>
-      <c r="F36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D37" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" t="s">
-        <v>76</v>
-      </c>
       <c r="F37" t="s">
-        <v>70</v>
-      </c>
-      <c r="G37" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F38" t="s">
         <v>70</v>
@@ -1219,10 +1225,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F39" t="s">
         <v>70</v>
@@ -1233,10 +1239,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F40" t="s">
         <v>70</v>
@@ -1247,10 +1253,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E41" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F41" t="s">
         <v>70</v>
@@ -1261,10 +1267,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E42" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F42" t="s">
         <v>70</v>
@@ -1275,10 +1281,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F43" t="s">
         <v>70</v>
@@ -1288,31 +1294,34 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="D44" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" t="s">
+        <v>84</v>
+      </c>
+      <c r="F44" t="s">
+        <v>70</v>
+      </c>
+      <c r="G44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>24</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>25</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>26</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>39</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>75</v>
-      </c>
-      <c r="F44" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D45" t="s">
-        <v>41</v>
-      </c>
-      <c r="E45" t="s">
-        <v>76</v>
       </c>
       <c r="F45" t="s">
         <v>62</v>
@@ -1320,10 +1329,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F46" t="s">
         <v>62</v>
@@ -1331,10 +1340,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F47" t="s">
         <v>62</v>
@@ -1342,10 +1351,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F48" t="s">
         <v>62</v>
@@ -1353,10 +1362,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E49" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F49" t="s">
         <v>62</v>
@@ -1364,10 +1373,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E50" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F50" t="s">
         <v>62</v>
@@ -1375,10 +1384,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E51" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F51" t="s">
         <v>62</v>
@@ -1386,59 +1395,70 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E52" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F52" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" t="s">
+        <v>88</v>
+      </c>
+      <c r="F53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
         <v>40</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" t="s">
         <v>57</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>89</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>10</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>85</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update formatFile and add StaffList.txt
</commit_message>
<xml_diff>
--- a/Data/FileFormat.xlsx
+++ b/Data/FileFormat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zerox\Code\Visual Studio\source\repos\KTLT\LabProject\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zerox\Code\Visual Studio\KTLT\Lab\GroupProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CB0107-B6BD-477F-9A0D-EA858E594FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5F10EF-EA58-4933-8058-13FC26C71103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -345,6 +345,21 @@
   </si>
   <si>
     <t>"Last name", last name</t>
+  </si>
+  <si>
+    <t>Staff List</t>
+  </si>
+  <si>
+    <t>StaffList.txt</t>
+  </si>
+  <si>
+    <t>"Number of staffs", staffList.size()</t>
+  </si>
+  <si>
+    <t>ID, password</t>
+  </si>
+  <si>
+    <t>Staff</t>
   </si>
 </sst>
 </file>
@@ -676,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1431,34 +1446,71 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" t="s">
+        <v>105</v>
+      </c>
+      <c r="F55" t="s">
+        <v>89</v>
+      </c>
+      <c r="G55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>40</v>
+      </c>
+      <c r="E56" t="s">
+        <v>106</v>
+      </c>
+      <c r="F56" t="s">
+        <v>89</v>
+      </c>
+      <c r="G56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>11</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B58" t="s">
         <v>20</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C58" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>21</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B59" t="s">
         <v>22</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C59" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>10</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B60" t="s">
         <v>85</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C60" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data to remove redundant data in Download and Upload function
</commit_message>
<xml_diff>
--- a/Data/FileFormat.xlsx
+++ b/Data/FileFormat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zerox\Code\Visual Studio\KTLT\Lab\GroupProject\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\GitHub\CSC10002-Course-Management\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5F10EF-EA58-4933-8058-13FC26C71103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA3C799-78DA-448D-B83A-F558BF2913C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -360,6 +360,27 @@
   </si>
   <si>
     <t>Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Download and Upload students in class (Class)</t>
+  </si>
+  <si>
+    <t>name+"_StudData.txt"</t>
+  </si>
+  <si>
+    <t>22CLC06_StudData.txt</t>
+  </si>
+  <si>
+    <t>Number of students</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>search</t>
   </si>
 </sst>
 </file>
@@ -691,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,7 +772,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
         <v>42</v>
@@ -1512,6 +1533,40 @@
       </c>
       <c r="C60" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" t="s">
+        <v>111</v>
+      </c>
+      <c r="D62" t="s">
+        <v>39</v>
+      </c>
+      <c r="E62" t="s">
+        <v>112</v>
+      </c>
+      <c r="F62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>40</v>
+      </c>
+      <c r="E63" t="s">
+        <v>113</v>
+      </c>
+      <c r="F63" t="s">
+        <v>114</v>
+      </c>
+      <c r="G63" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>